<commit_message>
trabalho no robo telegram para enviar ao solicitante
</commit_message>
<xml_diff>
--- a/Robo_PUT_ITUB4.xlsx
+++ b/Robo_PUT_ITUB4.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="80">
   <si>
     <t>STRIKE</t>
   </si>
@@ -160,88 +160,52 @@
     <t>ITUBM290</t>
   </si>
   <si>
-    <t>PETRM29</t>
-  </si>
-  <si>
     <t>ITUBM291</t>
   </si>
   <si>
     <t>ITUBM293</t>
   </si>
   <si>
-    <t>PETRM59</t>
-  </si>
-  <si>
     <t>ITUBM297</t>
   </si>
   <si>
     <t>ITUBM300</t>
   </si>
   <si>
-    <t>PETRM300</t>
-  </si>
-  <si>
     <t>ITUBM301</t>
   </si>
   <si>
     <t>ITUBM303</t>
   </si>
   <si>
-    <t>PETRM304</t>
-  </si>
-  <si>
-    <t>PETRM60</t>
-  </si>
-  <si>
     <t>ITUBM307</t>
   </si>
   <si>
-    <t>PETRM299</t>
-  </si>
-  <si>
     <t>ITUBM308</t>
   </si>
   <si>
-    <t>PETRM31</t>
-  </si>
-  <si>
     <t>ITUBM311</t>
   </si>
   <si>
     <t>ITUBM313</t>
   </si>
   <si>
-    <t>PETRM1</t>
-  </si>
-  <si>
     <t>ITUBM316</t>
   </si>
   <si>
-    <t>PETRM316</t>
-  </si>
-  <si>
     <t>ITUBM329</t>
   </si>
   <si>
-    <t>PETRM32</t>
-  </si>
-  <si>
     <t>ITUBM321</t>
   </si>
   <si>
     <t>ITUBM323</t>
   </si>
   <si>
-    <t>PETRM2</t>
-  </si>
-  <si>
     <t>ITUBM336</t>
   </si>
   <si>
     <t>ITUBM328</t>
-  </si>
-  <si>
-    <t>PETRM329</t>
   </si>
   <si>
     <t>ITUBM331</t>
@@ -647,7 +611,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I81"/>
+  <dimension ref="A1:I69"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -690,16 +654,16 @@
         <v>9</v>
       </c>
       <c r="C2" t="s">
-        <v>89</v>
+        <v>77</v>
       </c>
       <c r="D2" t="s">
-        <v>90</v>
+        <v>78</v>
       </c>
       <c r="E2">
-        <v>0.02</v>
+        <v>0.01</v>
       </c>
       <c r="F2">
-        <v>0.0013</v>
+        <v>0.0007</v>
       </c>
       <c r="G2">
         <v>-0.5</v>
@@ -708,7 +672,7 @@
         <v>0</v>
       </c>
       <c r="I2">
-        <v>2500</v>
+        <v>100</v>
       </c>
     </row>
     <row r="3" spans="1:9">
@@ -719,10 +683,10 @@
         <v>10</v>
       </c>
       <c r="C3" t="s">
-        <v>89</v>
+        <v>77</v>
       </c>
       <c r="D3" t="s">
-        <v>90</v>
+        <v>78</v>
       </c>
       <c r="E3">
         <v>0.03</v>
@@ -734,7 +698,7 @@
         <v>-0.38</v>
       </c>
       <c r="H3">
-        <v>0.2</v>
+        <v>0.17</v>
       </c>
       <c r="I3">
         <v>0</v>
@@ -748,10 +712,10 @@
         <v>11</v>
       </c>
       <c r="C4" t="s">
-        <v>89</v>
+        <v>77</v>
       </c>
       <c r="D4" t="s">
-        <v>90</v>
+        <v>78</v>
       </c>
       <c r="E4">
         <v>0.05</v>
@@ -763,7 +727,7 @@
         <v>-0.36</v>
       </c>
       <c r="H4">
-        <v>0.38</v>
+        <v>0.33</v>
       </c>
       <c r="I4">
         <v>0</v>
@@ -777,10 +741,10 @@
         <v>12</v>
       </c>
       <c r="C5" t="s">
-        <v>89</v>
+        <v>77</v>
       </c>
       <c r="D5" t="s">
-        <v>90</v>
+        <v>78</v>
       </c>
       <c r="E5">
         <v>0.12</v>
@@ -792,7 +756,7 @@
         <v>-0.34</v>
       </c>
       <c r="H5">
-        <v>0.67</v>
+        <v>0.59</v>
       </c>
       <c r="I5">
         <v>0</v>
@@ -806,10 +770,10 @@
         <v>13</v>
       </c>
       <c r="C6" t="s">
-        <v>89</v>
+        <v>77</v>
       </c>
       <c r="D6" t="s">
-        <v>90</v>
+        <v>78</v>
       </c>
       <c r="E6">
         <v>0.02</v>
@@ -821,7 +785,7 @@
         <v>-0.34</v>
       </c>
       <c r="H6">
-        <v>0.88</v>
+        <v>0.78</v>
       </c>
       <c r="I6">
         <v>0</v>
@@ -835,22 +799,22 @@
         <v>14</v>
       </c>
       <c r="C7" t="s">
-        <v>89</v>
+        <v>77</v>
       </c>
       <c r="D7" t="s">
-        <v>90</v>
+        <v>78</v>
       </c>
       <c r="E7">
-        <v>0.06</v>
+        <v>0.03</v>
       </c>
       <c r="F7">
-        <v>0.0029</v>
+        <v>0.0015</v>
       </c>
       <c r="G7">
         <v>-0.33</v>
       </c>
       <c r="H7">
-        <v>1.14</v>
+        <v>1.02</v>
       </c>
       <c r="I7">
         <v>0</v>
@@ -864,10 +828,10 @@
         <v>15</v>
       </c>
       <c r="C8" t="s">
-        <v>89</v>
+        <v>77</v>
       </c>
       <c r="D8" t="s">
-        <v>90</v>
+        <v>78</v>
       </c>
       <c r="E8">
         <v>0.07000000000000001</v>
@@ -879,7 +843,7 @@
         <v>-0.32</v>
       </c>
       <c r="H8">
-        <v>1.45</v>
+        <v>1.3</v>
       </c>
       <c r="I8">
         <v>0</v>
@@ -893,10 +857,10 @@
         <v>16</v>
       </c>
       <c r="C9" t="s">
-        <v>89</v>
+        <v>77</v>
       </c>
       <c r="D9" t="s">
-        <v>90</v>
+        <v>78</v>
       </c>
       <c r="E9">
         <v>0.06</v>
@@ -908,7 +872,7 @@
         <v>-0.31</v>
       </c>
       <c r="H9">
-        <v>1.84</v>
+        <v>1.66</v>
       </c>
       <c r="I9">
         <v>0</v>
@@ -922,10 +886,10 @@
         <v>17</v>
       </c>
       <c r="C10" t="s">
-        <v>89</v>
+        <v>77</v>
       </c>
       <c r="D10" t="s">
-        <v>90</v>
+        <v>78</v>
       </c>
       <c r="E10">
         <v>0.07000000000000001</v>
@@ -937,7 +901,7 @@
         <v>-0.3</v>
       </c>
       <c r="H10">
-        <v>2.31</v>
+        <v>2.08</v>
       </c>
       <c r="I10">
         <v>0</v>
@@ -951,10 +915,10 @@
         <v>18</v>
       </c>
       <c r="C11" t="s">
-        <v>89</v>
+        <v>77</v>
       </c>
       <c r="D11" t="s">
-        <v>90</v>
+        <v>78</v>
       </c>
       <c r="E11">
         <v>0.05</v>
@@ -966,7 +930,7 @@
         <v>-0.29</v>
       </c>
       <c r="H11">
-        <v>3.51</v>
+        <v>3.19</v>
       </c>
       <c r="I11">
         <v>0</v>
@@ -980,10 +944,10 @@
         <v>19</v>
       </c>
       <c r="C12" t="s">
-        <v>89</v>
+        <v>77</v>
       </c>
       <c r="D12" t="s">
-        <v>90</v>
+        <v>78</v>
       </c>
       <c r="E12">
         <v>0.05</v>
@@ -995,10 +959,10 @@
         <v>-0.28</v>
       </c>
       <c r="H12">
-        <v>4.27</v>
+        <v>3.89</v>
       </c>
       <c r="I12">
-        <v>0</v>
+        <v>1100</v>
       </c>
     </row>
     <row r="13" spans="1:9">
@@ -1009,25 +973,25 @@
         <v>20</v>
       </c>
       <c r="C13" t="s">
-        <v>89</v>
+        <v>77</v>
       </c>
       <c r="D13" t="s">
-        <v>90</v>
+        <v>78</v>
       </c>
       <c r="E13">
-        <v>0.05</v>
+        <v>0.06</v>
       </c>
       <c r="F13">
-        <v>0.0023</v>
+        <v>0.0027</v>
       </c>
       <c r="G13">
         <v>-0.27</v>
       </c>
       <c r="H13">
-        <v>5.14</v>
+        <v>4.7</v>
       </c>
       <c r="I13">
-        <v>0</v>
+        <v>60000</v>
       </c>
     </row>
     <row r="14" spans="1:9">
@@ -1038,25 +1002,25 @@
         <v>21</v>
       </c>
       <c r="C14" t="s">
-        <v>89</v>
+        <v>77</v>
       </c>
       <c r="D14" t="s">
-        <v>90</v>
+        <v>78</v>
       </c>
       <c r="E14">
-        <v>0.1</v>
+        <v>0.08</v>
       </c>
       <c r="F14">
-        <v>0.0045</v>
+        <v>0.0036</v>
       </c>
       <c r="G14">
         <v>-0.26</v>
       </c>
       <c r="H14">
-        <v>6.14</v>
+        <v>5.64</v>
       </c>
       <c r="I14">
-        <v>0</v>
+        <v>100</v>
       </c>
     </row>
     <row r="15" spans="1:9">
@@ -1067,25 +1031,25 @@
         <v>22</v>
       </c>
       <c r="C15" t="s">
-        <v>89</v>
+        <v>77</v>
       </c>
       <c r="D15" t="s">
-        <v>90</v>
+        <v>78</v>
       </c>
       <c r="E15">
-        <v>0.09</v>
+        <v>0.08</v>
       </c>
       <c r="F15">
-        <v>0.004</v>
+        <v>0.0035</v>
       </c>
       <c r="G15">
         <v>-0.25</v>
       </c>
       <c r="H15">
-        <v>7.27</v>
+        <v>6.69</v>
       </c>
       <c r="I15">
-        <v>0</v>
+        <v>400</v>
       </c>
     </row>
     <row r="16" spans="1:9">
@@ -1096,10 +1060,10 @@
         <v>23</v>
       </c>
       <c r="C16" t="s">
-        <v>89</v>
+        <v>77</v>
       </c>
       <c r="D16" t="s">
-        <v>90</v>
+        <v>78</v>
       </c>
       <c r="E16">
         <v>0.14</v>
@@ -1111,7 +1075,7 @@
         <v>-0.24</v>
       </c>
       <c r="H16">
-        <v>8.539999999999999</v>
+        <v>7.89</v>
       </c>
       <c r="I16">
         <v>0</v>
@@ -1125,10 +1089,10 @@
         <v>24</v>
       </c>
       <c r="C17" t="s">
-        <v>89</v>
+        <v>77</v>
       </c>
       <c r="D17" t="s">
-        <v>90</v>
+        <v>78</v>
       </c>
       <c r="E17">
         <v>0.1</v>
@@ -1140,7 +1104,7 @@
         <v>-0.24</v>
       </c>
       <c r="H17">
-        <v>9.949999999999999</v>
+        <v>9.220000000000001</v>
       </c>
       <c r="I17">
         <v>0</v>
@@ -1154,10 +1118,10 @@
         <v>25</v>
       </c>
       <c r="C18" t="s">
-        <v>89</v>
+        <v>77</v>
       </c>
       <c r="D18" t="s">
-        <v>90</v>
+        <v>78</v>
       </c>
       <c r="E18">
         <v>0.1</v>
@@ -1169,7 +1133,7 @@
         <v>-0.23</v>
       </c>
       <c r="H18">
-        <v>11.5</v>
+        <v>10.69</v>
       </c>
       <c r="I18">
         <v>0</v>
@@ -1183,10 +1147,10 @@
         <v>26</v>
       </c>
       <c r="C19" t="s">
-        <v>89</v>
+        <v>77</v>
       </c>
       <c r="D19" t="s">
-        <v>90</v>
+        <v>78</v>
       </c>
       <c r="E19">
         <v>0.12</v>
@@ -1198,7 +1162,7 @@
         <v>-0.22</v>
       </c>
       <c r="H19">
-        <v>13.2</v>
+        <v>12.31</v>
       </c>
       <c r="I19">
         <v>4000</v>
@@ -1212,25 +1176,25 @@
         <v>27</v>
       </c>
       <c r="C20" t="s">
-        <v>89</v>
+        <v>77</v>
       </c>
       <c r="D20" t="s">
-        <v>90</v>
+        <v>78</v>
       </c>
       <c r="E20">
-        <v>0.13</v>
+        <v>0.12</v>
       </c>
       <c r="F20">
-        <v>0.0054</v>
+        <v>0.005</v>
       </c>
       <c r="G20">
         <v>-0.21</v>
       </c>
       <c r="H20">
-        <v>15.05</v>
+        <v>14.07</v>
       </c>
       <c r="I20">
-        <v>5500</v>
+        <v>5700</v>
       </c>
     </row>
     <row r="21" spans="1:9">
@@ -1241,10 +1205,10 @@
         <v>28</v>
       </c>
       <c r="C21" t="s">
-        <v>89</v>
+        <v>77</v>
       </c>
       <c r="D21" t="s">
-        <v>90</v>
+        <v>78</v>
       </c>
       <c r="E21">
         <v>0.15</v>
@@ -1256,7 +1220,7 @@
         <v>-0.2</v>
       </c>
       <c r="H21">
-        <v>17.04</v>
+        <v>15.98</v>
       </c>
       <c r="I21">
         <v>10000</v>
@@ -1270,10 +1234,10 @@
         <v>29</v>
       </c>
       <c r="C22" t="s">
-        <v>89</v>
+        <v>77</v>
       </c>
       <c r="D22" t="s">
-        <v>90</v>
+        <v>78</v>
       </c>
       <c r="E22">
         <v>0.18</v>
@@ -1285,7 +1249,7 @@
         <v>-0.19</v>
       </c>
       <c r="H22">
-        <v>19.17</v>
+        <v>18.02</v>
       </c>
       <c r="I22">
         <v>0</v>
@@ -1299,10 +1263,10 @@
         <v>30</v>
       </c>
       <c r="C23" t="s">
-        <v>89</v>
+        <v>77</v>
       </c>
       <c r="D23" t="s">
-        <v>90</v>
+        <v>78</v>
       </c>
       <c r="E23">
         <v>0.18</v>
@@ -1314,7 +1278,7 @@
         <v>-0.19</v>
       </c>
       <c r="H23">
-        <v>21.43</v>
+        <v>20.2</v>
       </c>
       <c r="I23">
         <v>12800</v>
@@ -1328,25 +1292,25 @@
         <v>31</v>
       </c>
       <c r="C24" t="s">
-        <v>89</v>
+        <v>77</v>
       </c>
       <c r="D24" t="s">
-        <v>90</v>
+        <v>78</v>
       </c>
       <c r="E24">
-        <v>0.15</v>
+        <v>0.19</v>
       </c>
       <c r="F24">
-        <v>0.006</v>
+        <v>0.0076</v>
       </c>
       <c r="G24">
         <v>-0.18</v>
       </c>
       <c r="H24">
-        <v>23.81</v>
+        <v>22.5</v>
       </c>
       <c r="I24">
-        <v>0</v>
+        <v>200</v>
       </c>
     </row>
     <row r="25" spans="1:9">
@@ -1357,10 +1321,10 @@
         <v>32</v>
       </c>
       <c r="C25" t="s">
-        <v>89</v>
+        <v>77</v>
       </c>
       <c r="D25" t="s">
-        <v>90</v>
+        <v>78</v>
       </c>
       <c r="E25">
         <v>0.21</v>
@@ -1372,10 +1336,10 @@
         <v>-0.17</v>
       </c>
       <c r="H25">
-        <v>26.3</v>
+        <v>24.93</v>
       </c>
       <c r="I25">
-        <v>1000</v>
+        <v>1100</v>
       </c>
     </row>
     <row r="26" spans="1:9">
@@ -1386,10 +1350,10 @@
         <v>33</v>
       </c>
       <c r="C26" t="s">
-        <v>89</v>
+        <v>77</v>
       </c>
       <c r="D26" t="s">
-        <v>90</v>
+        <v>78</v>
       </c>
       <c r="E26">
         <v>0.22</v>
@@ -1401,7 +1365,7 @@
         <v>-0.16</v>
       </c>
       <c r="H26">
-        <v>28.9</v>
+        <v>27.45</v>
       </c>
       <c r="I26">
         <v>0</v>
@@ -1415,25 +1379,25 @@
         <v>34</v>
       </c>
       <c r="C27" t="s">
-        <v>89</v>
+        <v>77</v>
       </c>
       <c r="D27" t="s">
-        <v>90</v>
+        <v>78</v>
       </c>
       <c r="E27">
-        <v>0.24</v>
+        <v>0.25</v>
       </c>
       <c r="F27">
-        <v>0.0094</v>
+        <v>0.0098</v>
       </c>
       <c r="G27">
         <v>-0.15</v>
       </c>
       <c r="H27">
-        <v>31.58</v>
+        <v>30.07</v>
       </c>
       <c r="I27">
-        <v>0</v>
+        <v>4600</v>
       </c>
     </row>
     <row r="28" spans="1:9">
@@ -1444,25 +1408,25 @@
         <v>35</v>
       </c>
       <c r="C28" t="s">
-        <v>89</v>
+        <v>77</v>
       </c>
       <c r="D28" t="s">
-        <v>90</v>
+        <v>78</v>
       </c>
       <c r="E28">
-        <v>0.24</v>
+        <v>0.27</v>
       </c>
       <c r="F28">
-        <v>0.009299999999999999</v>
+        <v>0.0104</v>
       </c>
       <c r="G28">
         <v>-0.15</v>
       </c>
       <c r="H28">
-        <v>34.34</v>
+        <v>32.78</v>
       </c>
       <c r="I28">
-        <v>0</v>
+        <v>5000</v>
       </c>
     </row>
     <row r="29" spans="1:9">
@@ -1473,25 +1437,25 @@
         <v>36</v>
       </c>
       <c r="C29" t="s">
-        <v>89</v>
+        <v>77</v>
       </c>
       <c r="D29" t="s">
-        <v>90</v>
+        <v>78</v>
       </c>
       <c r="E29">
-        <v>0.31</v>
+        <v>0.3</v>
       </c>
       <c r="F29">
-        <v>0.0119</v>
+        <v>0.0115</v>
       </c>
       <c r="G29">
         <v>-0.14</v>
       </c>
       <c r="H29">
-        <v>37.15</v>
+        <v>35.54</v>
       </c>
       <c r="I29">
-        <v>30900</v>
+        <v>48500</v>
       </c>
     </row>
     <row r="30" spans="1:9">
@@ -1502,25 +1466,25 @@
         <v>37</v>
       </c>
       <c r="C30" t="s">
-        <v>89</v>
+        <v>77</v>
       </c>
       <c r="D30" t="s">
-        <v>90</v>
+        <v>78</v>
       </c>
       <c r="E30">
-        <v>0.31</v>
+        <v>0.33</v>
       </c>
       <c r="F30">
-        <v>0.0118</v>
+        <v>0.0125</v>
       </c>
       <c r="G30">
         <v>-0.13</v>
       </c>
       <c r="H30">
-        <v>40.01</v>
+        <v>38.36</v>
       </c>
       <c r="I30">
-        <v>0</v>
+        <v>400</v>
       </c>
     </row>
     <row r="31" spans="1:9">
@@ -1531,25 +1495,25 @@
         <v>38</v>
       </c>
       <c r="C31" t="s">
-        <v>89</v>
+        <v>77</v>
       </c>
       <c r="D31" t="s">
-        <v>90</v>
+        <v>78</v>
       </c>
       <c r="E31">
-        <v>0.41</v>
+        <v>0.37</v>
       </c>
       <c r="F31">
-        <v>0.0154</v>
+        <v>0.0139</v>
       </c>
       <c r="G31">
         <v>-0.12</v>
       </c>
       <c r="H31">
-        <v>42.89</v>
+        <v>41.22</v>
       </c>
       <c r="I31">
-        <v>3200</v>
+        <v>60200</v>
       </c>
     </row>
     <row r="32" spans="1:9">
@@ -1560,25 +1524,25 @@
         <v>39</v>
       </c>
       <c r="C32" t="s">
-        <v>89</v>
+        <v>77</v>
       </c>
       <c r="D32" t="s">
-        <v>90</v>
+        <v>78</v>
       </c>
       <c r="E32">
-        <v>0.44</v>
+        <v>0.41</v>
       </c>
       <c r="F32">
-        <v>0.0164</v>
+        <v>0.0153</v>
       </c>
       <c r="G32">
         <v>-0.11</v>
       </c>
       <c r="H32">
-        <v>45.78</v>
+        <v>44.09</v>
       </c>
       <c r="I32">
-        <v>31900</v>
+        <v>81000</v>
       </c>
     </row>
     <row r="33" spans="1:9">
@@ -1589,10 +1553,10 @@
         <v>40</v>
       </c>
       <c r="C33" t="s">
-        <v>89</v>
+        <v>77</v>
       </c>
       <c r="D33" t="s">
-        <v>90</v>
+        <v>78</v>
       </c>
       <c r="E33">
         <v>0.47</v>
@@ -1604,10 +1568,10 @@
         <v>-0.1</v>
       </c>
       <c r="H33">
-        <v>48.67</v>
+        <v>46.97</v>
       </c>
       <c r="I33">
-        <v>44600</v>
+        <v>56200</v>
       </c>
     </row>
     <row r="34" spans="1:9">
@@ -1618,25 +1582,25 @@
         <v>41</v>
       </c>
       <c r="C34" t="s">
-        <v>89</v>
+        <v>77</v>
       </c>
       <c r="D34" t="s">
-        <v>90</v>
+        <v>78</v>
       </c>
       <c r="E34">
-        <v>0.52</v>
+        <v>0.53</v>
       </c>
       <c r="F34">
-        <v>0.019</v>
+        <v>0.0194</v>
       </c>
       <c r="G34">
         <v>-0.1</v>
       </c>
       <c r="H34">
-        <v>51.54</v>
+        <v>49.84</v>
       </c>
       <c r="I34">
-        <v>10600</v>
+        <v>8298300</v>
       </c>
     </row>
     <row r="35" spans="1:9">
@@ -1647,25 +1611,25 @@
         <v>42</v>
       </c>
       <c r="C35" t="s">
-        <v>89</v>
+        <v>77</v>
       </c>
       <c r="D35" t="s">
-        <v>90</v>
+        <v>78</v>
       </c>
       <c r="E35">
-        <v>0.68</v>
+        <v>0.57</v>
       </c>
       <c r="F35">
-        <v>0.0246</v>
+        <v>0.0206</v>
       </c>
       <c r="G35">
         <v>-0.09</v>
       </c>
       <c r="H35">
-        <v>54.38</v>
+        <v>52.68</v>
       </c>
       <c r="I35">
-        <v>4000</v>
+        <v>4100</v>
       </c>
     </row>
     <row r="36" spans="1:9">
@@ -1676,25 +1640,25 @@
         <v>43</v>
       </c>
       <c r="C36" t="s">
-        <v>89</v>
+        <v>77</v>
       </c>
       <c r="D36" t="s">
-        <v>90</v>
+        <v>78</v>
       </c>
       <c r="E36">
-        <v>0.62</v>
+        <v>0.59</v>
       </c>
       <c r="F36">
-        <v>0.0223</v>
+        <v>0.0212</v>
       </c>
       <c r="G36">
         <v>-0.08</v>
       </c>
       <c r="H36">
-        <v>57.17</v>
+        <v>55.48</v>
       </c>
       <c r="I36">
-        <v>42700</v>
+        <v>125800</v>
       </c>
     </row>
     <row r="37" spans="1:9">
@@ -1705,25 +1669,25 @@
         <v>44</v>
       </c>
       <c r="C37" t="s">
-        <v>89</v>
+        <v>77</v>
       </c>
       <c r="D37" t="s">
-        <v>90</v>
+        <v>78</v>
       </c>
       <c r="E37">
-        <v>0.71</v>
+        <v>0.66</v>
       </c>
       <c r="F37">
-        <v>0.0253</v>
+        <v>0.0235</v>
       </c>
       <c r="G37">
         <v>-0.07000000000000001</v>
       </c>
       <c r="H37">
-        <v>59.9</v>
+        <v>58.23</v>
       </c>
       <c r="I37">
-        <v>0</v>
+        <v>33000</v>
       </c>
     </row>
     <row r="38" spans="1:9">
@@ -1734,10 +1698,10 @@
         <v>45</v>
       </c>
       <c r="C38" t="s">
-        <v>89</v>
+        <v>77</v>
       </c>
       <c r="D38" t="s">
-        <v>90</v>
+        <v>78</v>
       </c>
       <c r="E38">
         <v>0.76</v>
@@ -1749,10 +1713,10 @@
         <v>-0.06</v>
       </c>
       <c r="H38">
-        <v>62.56</v>
+        <v>60.92</v>
       </c>
       <c r="I38">
-        <v>41900</v>
+        <v>48500</v>
       </c>
     </row>
     <row r="39" spans="1:9">
@@ -1763,25 +1727,25 @@
         <v>46</v>
       </c>
       <c r="C39" t="s">
-        <v>89</v>
+        <v>77</v>
       </c>
       <c r="D39" t="s">
-        <v>90</v>
+        <v>78</v>
       </c>
       <c r="E39">
-        <v>0.95</v>
+        <v>0.83</v>
       </c>
       <c r="F39">
-        <v>0.0332</v>
+        <v>0.029</v>
       </c>
       <c r="G39">
         <v>-0.05</v>
       </c>
       <c r="H39">
-        <v>65.13</v>
+        <v>63.54</v>
       </c>
       <c r="I39">
-        <v>19000</v>
+        <v>19100</v>
       </c>
     </row>
     <row r="40" spans="1:9">
@@ -1792,396 +1756,399 @@
         <v>47</v>
       </c>
       <c r="C40" t="s">
-        <v>89</v>
+        <v>77</v>
       </c>
       <c r="D40" t="s">
-        <v>90</v>
+        <v>78</v>
       </c>
       <c r="E40">
-        <v>0.9399999999999999</v>
+        <v>0.9</v>
       </c>
       <c r="F40">
-        <v>0.0326</v>
+        <v>0.0312</v>
       </c>
       <c r="G40">
         <v>-0.05</v>
       </c>
       <c r="H40">
-        <v>67.62</v>
+        <v>66.06999999999999</v>
       </c>
       <c r="I40">
-        <v>21700</v>
+        <v>21900</v>
       </c>
     </row>
     <row r="41" spans="1:9">
       <c r="A41">
-        <v>29</v>
+        <v>29.11</v>
       </c>
       <c r="B41" t="s">
         <v>48</v>
       </c>
       <c r="C41" t="s">
-        <v>89</v>
+        <v>77</v>
       </c>
       <c r="D41" t="s">
-        <v>90</v>
+        <v>78</v>
       </c>
       <c r="E41">
-        <v>2.56</v>
+        <v>0.97</v>
       </c>
       <c r="F41">
-        <v>0.0883</v>
+        <v>0.0333</v>
       </c>
       <c r="G41">
         <v>-0.04</v>
       </c>
       <c r="H41">
-        <v>68.97</v>
+        <v>68.51000000000001</v>
       </c>
       <c r="I41">
-        <v>319900</v>
+        <v>7700</v>
       </c>
     </row>
     <row r="42" spans="1:9">
       <c r="A42">
-        <v>29.11</v>
+        <v>29.36</v>
       </c>
       <c r="B42" t="s">
         <v>49</v>
       </c>
       <c r="C42" t="s">
-        <v>89</v>
+        <v>77</v>
       </c>
       <c r="D42" t="s">
-        <v>90</v>
+        <v>78</v>
       </c>
       <c r="E42">
-        <v>1.06</v>
+        <v>1.15</v>
       </c>
       <c r="F42">
-        <v>0.0364</v>
+        <v>0.0392</v>
       </c>
       <c r="G42">
-        <v>-0.04</v>
+        <v>-0.03</v>
       </c>
       <c r="H42">
-        <v>70.01000000000001</v>
+        <v>70.84999999999999</v>
       </c>
       <c r="I42">
-        <v>6600</v>
+        <v>4000</v>
       </c>
     </row>
     <row r="43" spans="1:9">
       <c r="A43">
-        <v>29.36</v>
+        <v>29.61</v>
       </c>
       <c r="B43" t="s">
         <v>50</v>
       </c>
       <c r="C43" t="s">
-        <v>89</v>
+        <v>77</v>
       </c>
       <c r="D43" t="s">
-        <v>90</v>
+        <v>78</v>
       </c>
       <c r="E43">
-        <v>1.16</v>
+        <v>1.18</v>
       </c>
       <c r="F43">
-        <v>0.0395</v>
+        <v>0.0399</v>
       </c>
       <c r="G43">
-        <v>-0.03</v>
+        <v>-0.02</v>
       </c>
       <c r="H43">
-        <v>72.3</v>
+        <v>73.09</v>
       </c>
       <c r="I43">
-        <v>1300</v>
+        <v>32500</v>
       </c>
     </row>
     <row r="44" spans="1:9">
       <c r="A44">
-        <v>29.5</v>
+        <v>29.86</v>
       </c>
       <c r="B44" t="s">
         <v>51</v>
       </c>
       <c r="C44" t="s">
-        <v>89</v>
+        <v>77</v>
       </c>
       <c r="D44" t="s">
-        <v>90</v>
+        <v>78</v>
       </c>
       <c r="E44">
-        <v>3.07</v>
+        <v>1.26</v>
       </c>
       <c r="F44">
-        <v>0.1041</v>
+        <v>0.0422</v>
       </c>
       <c r="G44">
-        <v>-0.03</v>
+        <v>-0.01</v>
       </c>
       <c r="H44">
-        <v>73.54000000000001</v>
+        <v>75.22</v>
       </c>
       <c r="I44">
-        <v>66100</v>
+        <v>109900</v>
       </c>
     </row>
     <row r="45" spans="1:9">
       <c r="A45">
-        <v>29.61</v>
+        <v>30.11</v>
       </c>
       <c r="B45" t="s">
         <v>52</v>
       </c>
       <c r="C45" t="s">
-        <v>89</v>
+        <v>77</v>
       </c>
       <c r="D45" t="s">
-        <v>90</v>
+        <v>78</v>
       </c>
       <c r="E45">
-        <v>1.19</v>
+        <v>1.38</v>
       </c>
       <c r="F45">
-        <v>0.0402</v>
+        <v>0.0458</v>
       </c>
       <c r="G45">
-        <v>-0.02</v>
+        <v>-0</v>
       </c>
       <c r="H45">
-        <v>74.48</v>
+        <v>77.23999999999999</v>
       </c>
       <c r="I45">
-        <v>0</v>
+        <v>48100</v>
       </c>
     </row>
     <row r="46" spans="1:9">
       <c r="A46">
-        <v>29.86</v>
+        <v>30.36</v>
       </c>
       <c r="B46" t="s">
         <v>53</v>
       </c>
       <c r="C46" t="s">
-        <v>89</v>
+        <v>77</v>
       </c>
       <c r="D46" t="s">
-        <v>90</v>
+        <v>78</v>
       </c>
       <c r="E46">
-        <v>1.4</v>
+        <v>1.48</v>
       </c>
       <c r="F46">
-        <v>0.0469</v>
+        <v>0.0487</v>
       </c>
       <c r="G46">
-        <v>-0.01</v>
+        <v>0</v>
       </c>
       <c r="H46">
-        <v>76.55</v>
+        <v>79.15000000000001</v>
       </c>
       <c r="I46">
-        <v>106700</v>
+        <v>21500</v>
       </c>
     </row>
     <row r="47" spans="1:9">
       <c r="A47">
-        <v>30</v>
+        <v>30.61</v>
       </c>
       <c r="B47" t="s">
         <v>54</v>
       </c>
       <c r="C47" t="s">
-        <v>89</v>
+        <v>77</v>
       </c>
       <c r="D47" t="s">
-        <v>90</v>
+        <v>78</v>
       </c>
       <c r="E47">
-        <v>3.28</v>
+        <v>1.6</v>
       </c>
       <c r="F47">
-        <v>0.1093</v>
+        <v>0.0523</v>
       </c>
       <c r="G47">
-        <v>-0.01</v>
+        <v>0.01</v>
       </c>
       <c r="H47">
-        <v>77.66</v>
+        <v>80.94</v>
       </c>
       <c r="I47">
-        <v>60800</v>
+        <v>30200</v>
       </c>
     </row>
     <row r="48" spans="1:9">
       <c r="A48">
-        <v>30.11</v>
+        <v>30.86</v>
       </c>
       <c r="B48" t="s">
         <v>55</v>
       </c>
       <c r="C48" t="s">
-        <v>89</v>
+        <v>77</v>
       </c>
       <c r="D48" t="s">
-        <v>90</v>
+        <v>78</v>
       </c>
       <c r="E48">
-        <v>1.45</v>
+        <v>1.75</v>
       </c>
       <c r="F48">
-        <v>0.0482</v>
+        <v>0.0567</v>
       </c>
       <c r="G48">
-        <v>-0</v>
+        <v>0.02</v>
       </c>
       <c r="H48">
-        <v>78.51000000000001</v>
+        <v>82.63</v>
       </c>
       <c r="I48">
-        <v>19600</v>
+        <v>236500</v>
       </c>
     </row>
     <row r="49" spans="1:9">
       <c r="A49">
-        <v>30.36</v>
+        <v>31.11</v>
       </c>
       <c r="B49" t="s">
         <v>56</v>
       </c>
       <c r="C49" t="s">
-        <v>89</v>
+        <v>77</v>
       </c>
       <c r="D49" t="s">
-        <v>90</v>
+        <v>78</v>
       </c>
       <c r="E49">
-        <v>1.39</v>
+        <v>1.99</v>
       </c>
       <c r="F49">
-        <v>0.0458</v>
+        <v>0.064</v>
       </c>
       <c r="G49">
-        <v>0</v>
+        <v>0.03</v>
       </c>
       <c r="H49">
-        <v>80.34999999999999</v>
+        <v>84.2</v>
       </c>
       <c r="I49">
-        <v>0</v>
+        <v>1200</v>
       </c>
     </row>
     <row r="50" spans="1:9">
       <c r="A50">
-        <v>30.5</v>
+        <v>31.36</v>
       </c>
       <c r="B50" t="s">
         <v>57</v>
       </c>
       <c r="C50" t="s">
-        <v>89</v>
+        <v>77</v>
       </c>
       <c r="D50" t="s">
-        <v>90</v>
+        <v>78</v>
       </c>
       <c r="E50">
-        <v>3.66</v>
+        <v>2.1</v>
       </c>
       <c r="F50">
-        <v>0.12</v>
+        <v>0.067</v>
       </c>
       <c r="G50">
-        <v>0.01</v>
+        <v>0.04</v>
       </c>
       <c r="H50">
-        <v>81.34</v>
+        <v>85.67</v>
       </c>
       <c r="I50">
-        <v>20000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="51" spans="1:9">
       <c r="A51">
-        <v>30.5</v>
+        <v>31.61</v>
       </c>
       <c r="B51" t="s">
         <v>58</v>
       </c>
       <c r="C51" t="s">
-        <v>89</v>
+        <v>77</v>
       </c>
       <c r="D51" t="s">
-        <v>90</v>
-      </c>
-      <c r="E51" t="s">
-        <v>91</v>
+        <v>78</v>
+      </c>
+      <c r="E51">
+        <v>2.22</v>
+      </c>
+      <c r="F51">
+        <v>0.0702</v>
       </c>
       <c r="G51">
-        <v>0.01</v>
+        <v>0.04</v>
       </c>
       <c r="H51">
-        <v>81.34</v>
-      </c>
-      <c r="I51" t="s">
-        <v>91</v>
+        <v>87.03</v>
+      </c>
+      <c r="I51">
+        <v>2800</v>
       </c>
     </row>
     <row r="52" spans="1:9">
       <c r="A52">
-        <v>30.61</v>
+        <v>31.86</v>
       </c>
       <c r="B52" t="s">
         <v>59</v>
       </c>
       <c r="C52" t="s">
-        <v>89</v>
+        <v>77</v>
       </c>
       <c r="D52" t="s">
-        <v>90</v>
+        <v>78</v>
       </c>
       <c r="E52">
-        <v>1.5</v>
+        <v>2.6</v>
       </c>
       <c r="F52">
-        <v>0.049</v>
+        <v>0.08160000000000001</v>
       </c>
       <c r="G52">
-        <v>0.01</v>
+        <v>0.05</v>
       </c>
       <c r="H52">
-        <v>82.09</v>
+        <v>88.29000000000001</v>
       </c>
       <c r="I52">
-        <v>0</v>
+        <v>3000</v>
       </c>
     </row>
     <row r="53" spans="1:9">
       <c r="A53">
-        <v>30.75</v>
+        <v>32.11</v>
       </c>
       <c r="B53" t="s">
         <v>60</v>
       </c>
       <c r="C53" t="s">
-        <v>89</v>
+        <v>77</v>
       </c>
       <c r="D53" t="s">
-        <v>90</v>
+        <v>78</v>
       </c>
       <c r="E53">
-        <v>4.24</v>
+        <v>2.41</v>
       </c>
       <c r="F53">
-        <v>0.1379</v>
+        <v>0.0751</v>
       </c>
       <c r="G53">
-        <v>0.02</v>
+        <v>0.06</v>
       </c>
       <c r="H53">
-        <v>83.01000000000001</v>
+        <v>89.45</v>
       </c>
       <c r="I53">
         <v>0</v>
@@ -2189,115 +2156,115 @@
     </row>
     <row r="54" spans="1:9">
       <c r="A54">
-        <v>30.86</v>
+        <v>32.36</v>
       </c>
       <c r="B54" t="s">
         <v>61</v>
       </c>
       <c r="C54" t="s">
-        <v>89</v>
+        <v>77</v>
       </c>
       <c r="D54" t="s">
-        <v>90</v>
+        <v>78</v>
       </c>
       <c r="E54">
-        <v>1.92</v>
+        <v>2.88</v>
       </c>
       <c r="F54">
-        <v>0.0622</v>
+        <v>0.089</v>
       </c>
       <c r="G54">
-        <v>0.02</v>
+        <v>0.07000000000000001</v>
       </c>
       <c r="H54">
-        <v>83.7</v>
+        <v>90.52</v>
       </c>
       <c r="I54">
-        <v>170200</v>
+        <v>200</v>
       </c>
     </row>
     <row r="55" spans="1:9">
       <c r="A55">
-        <v>31</v>
+        <v>32.61</v>
       </c>
       <c r="B55" t="s">
         <v>62</v>
       </c>
       <c r="C55" t="s">
-        <v>89</v>
+        <v>77</v>
       </c>
       <c r="D55" t="s">
-        <v>90</v>
+        <v>78</v>
       </c>
       <c r="E55">
-        <v>4.05</v>
+        <v>7.71</v>
       </c>
       <c r="F55">
-        <v>0.1306</v>
+        <v>0.2364</v>
       </c>
       <c r="G55">
-        <v>0.02</v>
+        <v>0.08</v>
       </c>
       <c r="H55">
-        <v>84.56</v>
+        <v>91.5</v>
       </c>
       <c r="I55">
-        <v>3300</v>
+        <v>0</v>
       </c>
     </row>
     <row r="56" spans="1:9">
       <c r="A56">
-        <v>31.11</v>
+        <v>32.86</v>
       </c>
       <c r="B56" t="s">
         <v>63</v>
       </c>
       <c r="C56" t="s">
-        <v>89</v>
+        <v>77</v>
       </c>
       <c r="D56" t="s">
-        <v>90</v>
+        <v>78</v>
       </c>
       <c r="E56">
-        <v>2.1</v>
+        <v>3.4</v>
       </c>
       <c r="F56">
-        <v>0.0675</v>
+        <v>0.1035</v>
       </c>
       <c r="G56">
-        <v>0.03</v>
+        <v>0.09</v>
       </c>
       <c r="H56">
-        <v>85.20999999999999</v>
+        <v>92.39</v>
       </c>
       <c r="I56">
-        <v>100</v>
+        <v>0</v>
       </c>
     </row>
     <row r="57" spans="1:9">
       <c r="A57">
-        <v>31.36</v>
+        <v>33.11</v>
       </c>
       <c r="B57" t="s">
         <v>64</v>
       </c>
       <c r="C57" t="s">
-        <v>89</v>
+        <v>77</v>
       </c>
       <c r="D57" t="s">
-        <v>90</v>
+        <v>78</v>
       </c>
       <c r="E57">
-        <v>2.1</v>
+        <v>0</v>
       </c>
       <c r="F57">
-        <v>0.067</v>
+        <v>0</v>
       </c>
       <c r="G57">
-        <v>0.04</v>
+        <v>0.09</v>
       </c>
       <c r="H57">
-        <v>86.62</v>
+        <v>93.20999999999999</v>
       </c>
       <c r="I57">
         <v>0</v>
@@ -2305,28 +2272,28 @@
     </row>
     <row r="58" spans="1:9">
       <c r="A58">
-        <v>31.5</v>
+        <v>33.61</v>
       </c>
       <c r="B58" t="s">
         <v>65</v>
       </c>
       <c r="C58" t="s">
-        <v>89</v>
+        <v>77</v>
       </c>
       <c r="D58" t="s">
-        <v>90</v>
+        <v>78</v>
       </c>
       <c r="E58">
-        <v>8.460000000000001</v>
+        <v>0</v>
       </c>
       <c r="F58">
-        <v>0.2686</v>
+        <v>0</v>
       </c>
       <c r="G58">
-        <v>0.04</v>
+        <v>0.11</v>
       </c>
       <c r="H58">
-        <v>87.34999999999999</v>
+        <v>94.62</v>
       </c>
       <c r="I58">
         <v>0</v>
@@ -2334,28 +2301,28 @@
     </row>
     <row r="59" spans="1:9">
       <c r="A59">
-        <v>31.61</v>
+        <v>34.11</v>
       </c>
       <c r="B59" t="s">
         <v>66</v>
       </c>
       <c r="C59" t="s">
-        <v>89</v>
+        <v>77</v>
       </c>
       <c r="D59" t="s">
-        <v>90</v>
+        <v>78</v>
       </c>
       <c r="E59">
-        <v>2.54</v>
+        <v>0</v>
       </c>
       <c r="F59">
-        <v>0.0804</v>
+        <v>0</v>
       </c>
       <c r="G59">
-        <v>0.04</v>
+        <v>0.13</v>
       </c>
       <c r="H59">
-        <v>87.91</v>
+        <v>95.77</v>
       </c>
       <c r="I59">
         <v>0</v>
@@ -2363,144 +2330,144 @@
     </row>
     <row r="60" spans="1:9">
       <c r="A60">
-        <v>31.75</v>
+        <v>34.36</v>
       </c>
       <c r="B60" t="s">
         <v>67</v>
       </c>
       <c r="C60" t="s">
-        <v>89</v>
+        <v>77</v>
       </c>
       <c r="D60" t="s">
-        <v>90</v>
+        <v>78</v>
       </c>
       <c r="E60">
-        <v>4.68</v>
+        <v>5.9</v>
       </c>
       <c r="F60">
-        <v>0.1474</v>
+        <v>0.1717</v>
       </c>
       <c r="G60">
-        <v>0.05</v>
+        <v>0.14</v>
       </c>
       <c r="H60">
-        <v>88.59999999999999</v>
+        <v>96.26000000000001</v>
       </c>
       <c r="I60">
-        <v>112300</v>
+        <v>0</v>
       </c>
     </row>
     <row r="61" spans="1:9">
       <c r="A61">
-        <v>31.86</v>
+        <v>34.86</v>
       </c>
       <c r="B61" t="s">
         <v>68</v>
       </c>
       <c r="C61" t="s">
-        <v>89</v>
+        <v>77</v>
       </c>
       <c r="D61" t="s">
-        <v>90</v>
+        <v>78</v>
       </c>
       <c r="E61">
-        <v>2.6</v>
+        <v>5.07</v>
       </c>
       <c r="F61">
-        <v>0.08160000000000001</v>
+        <v>0.1454</v>
       </c>
       <c r="G61">
-        <v>0.05</v>
+        <v>0.15</v>
       </c>
       <c r="H61">
-        <v>89.11</v>
+        <v>97.09999999999999</v>
       </c>
       <c r="I61">
-        <v>3000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="62" spans="1:9">
       <c r="A62">
-        <v>32</v>
+        <v>35.11</v>
       </c>
       <c r="B62" t="s">
         <v>69</v>
       </c>
       <c r="C62" t="s">
-        <v>89</v>
+        <v>77</v>
       </c>
       <c r="D62" t="s">
-        <v>90</v>
+        <v>78</v>
       </c>
       <c r="E62">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="F62">
-        <v>0.1562</v>
+        <v>0</v>
       </c>
       <c r="G62">
-        <v>0.06</v>
+        <v>0.16</v>
       </c>
       <c r="H62">
-        <v>89.73999999999999</v>
+        <v>97.45</v>
       </c>
       <c r="I62">
-        <v>200</v>
+        <v>0</v>
       </c>
     </row>
     <row r="63" spans="1:9">
       <c r="A63">
-        <v>32.11</v>
+        <v>35.61</v>
       </c>
       <c r="B63" t="s">
         <v>70</v>
       </c>
       <c r="C63" t="s">
-        <v>89</v>
+        <v>77</v>
       </c>
       <c r="D63" t="s">
-        <v>90</v>
+        <v>78</v>
       </c>
       <c r="E63">
-        <v>2.41</v>
+        <v>5.3</v>
       </c>
       <c r="F63">
-        <v>0.0751</v>
+        <v>0.1488</v>
       </c>
       <c r="G63">
-        <v>0.06</v>
+        <v>0.18</v>
       </c>
       <c r="H63">
-        <v>90.20999999999999</v>
+        <v>98.04000000000001</v>
       </c>
       <c r="I63">
-        <v>0</v>
+        <v>5000</v>
       </c>
     </row>
     <row r="64" spans="1:9">
       <c r="A64">
-        <v>32.36</v>
+        <v>36.86</v>
       </c>
       <c r="B64" t="s">
         <v>71</v>
       </c>
       <c r="C64" t="s">
-        <v>89</v>
+        <v>77</v>
       </c>
       <c r="D64" t="s">
-        <v>90</v>
+        <v>78</v>
       </c>
       <c r="E64">
-        <v>2.85</v>
+        <v>0</v>
       </c>
       <c r="F64">
-        <v>0.0881</v>
+        <v>0</v>
       </c>
       <c r="G64">
-        <v>0.07000000000000001</v>
+        <v>0.22</v>
       </c>
       <c r="H64">
-        <v>91.22</v>
+        <v>99.02</v>
       </c>
       <c r="I64">
         <v>0</v>
@@ -2508,54 +2475,57 @@
     </row>
     <row r="65" spans="1:9">
       <c r="A65">
-        <v>32.5</v>
+        <v>37.36</v>
       </c>
       <c r="B65" t="s">
         <v>72</v>
       </c>
       <c r="C65" t="s">
-        <v>89</v>
+        <v>77</v>
       </c>
       <c r="D65" t="s">
-        <v>90</v>
-      </c>
-      <c r="E65" t="s">
-        <v>91</v>
+        <v>78</v>
+      </c>
+      <c r="E65">
+        <v>0</v>
+      </c>
+      <c r="F65">
+        <v>0</v>
       </c>
       <c r="G65">
-        <v>0.07000000000000001</v>
+        <v>0.23</v>
       </c>
       <c r="H65">
-        <v>91.75</v>
-      </c>
-      <c r="I65" t="s">
-        <v>91</v>
+        <v>99.26000000000001</v>
+      </c>
+      <c r="I65">
+        <v>0</v>
       </c>
     </row>
     <row r="66" spans="1:9">
       <c r="A66">
-        <v>32.61</v>
+        <v>37.86</v>
       </c>
       <c r="B66" t="s">
         <v>73</v>
       </c>
       <c r="C66" t="s">
-        <v>89</v>
+        <v>77</v>
       </c>
       <c r="D66" t="s">
-        <v>90</v>
+        <v>78</v>
       </c>
       <c r="E66">
-        <v>7.71</v>
+        <v>0</v>
       </c>
       <c r="F66">
-        <v>0.2364</v>
+        <v>0</v>
       </c>
       <c r="G66">
-        <v>0.08</v>
+        <v>0.25</v>
       </c>
       <c r="H66">
-        <v>92.14</v>
+        <v>99.45</v>
       </c>
       <c r="I66">
         <v>0</v>
@@ -2563,28 +2533,28 @@
     </row>
     <row r="67" spans="1:9">
       <c r="A67">
-        <v>32.86</v>
+        <v>38.36</v>
       </c>
       <c r="B67" t="s">
         <v>74</v>
       </c>
       <c r="C67" t="s">
-        <v>89</v>
+        <v>77</v>
       </c>
       <c r="D67" t="s">
-        <v>90</v>
+        <v>78</v>
       </c>
       <c r="E67">
-        <v>3.4</v>
+        <v>0</v>
       </c>
       <c r="F67">
-        <v>0.1035</v>
+        <v>0</v>
       </c>
       <c r="G67">
-        <v>0.09</v>
+        <v>0.27</v>
       </c>
       <c r="H67">
-        <v>92.98</v>
+        <v>99.59</v>
       </c>
       <c r="I67">
         <v>0</v>
@@ -2592,405 +2562,57 @@
     </row>
     <row r="68" spans="1:9">
       <c r="A68">
-        <v>33</v>
+        <v>38.86</v>
       </c>
       <c r="B68" t="s">
         <v>75</v>
       </c>
       <c r="C68" t="s">
-        <v>89</v>
+        <v>77</v>
       </c>
       <c r="D68" t="s">
-        <v>90</v>
+        <v>78</v>
       </c>
       <c r="E68">
-        <v>5.85</v>
+        <v>0</v>
       </c>
       <c r="F68">
-        <v>0.1773</v>
+        <v>0</v>
       </c>
       <c r="G68">
-        <v>0.09</v>
+        <v>0.28</v>
       </c>
       <c r="H68">
-        <v>93.42</v>
+        <v>99.7</v>
       </c>
       <c r="I68">
-        <v>34000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="69" spans="1:9">
       <c r="A69">
-        <v>33.11</v>
+        <v>43.11</v>
       </c>
       <c r="B69" t="s">
         <v>76</v>
       </c>
       <c r="C69" t="s">
-        <v>89</v>
+        <v>77</v>
       </c>
       <c r="D69" t="s">
-        <v>90</v>
-      </c>
-      <c r="E69">
-        <v>0</v>
-      </c>
-      <c r="F69">
-        <v>0</v>
+        <v>78</v>
+      </c>
+      <c r="E69" t="s">
+        <v>79</v>
       </c>
       <c r="G69">
-        <v>0.09</v>
+        <v>0.42</v>
       </c>
       <c r="H69">
-        <v>93.75</v>
-      </c>
-      <c r="I69">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="70" spans="1:9">
-      <c r="A70">
-        <v>33.61</v>
-      </c>
-      <c r="B70" t="s">
-        <v>77</v>
-      </c>
-      <c r="C70" t="s">
-        <v>89</v>
-      </c>
-      <c r="D70" t="s">
-        <v>90</v>
-      </c>
-      <c r="E70">
-        <v>0</v>
-      </c>
-      <c r="F70">
-        <v>0</v>
-      </c>
-      <c r="G70">
-        <v>0.11</v>
-      </c>
-      <c r="H70">
-        <v>95.06999999999999</v>
-      </c>
-      <c r="I70">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="71" spans="1:9">
-      <c r="A71">
-        <v>34.11</v>
-      </c>
-      <c r="B71" t="s">
-        <v>78</v>
-      </c>
-      <c r="C71" t="s">
-        <v>89</v>
-      </c>
-      <c r="D71" t="s">
-        <v>90</v>
-      </c>
-      <c r="E71">
-        <v>0</v>
-      </c>
-      <c r="F71">
-        <v>0</v>
-      </c>
-      <c r="G71">
-        <v>0.13</v>
-      </c>
-      <c r="H71">
-        <v>96.14</v>
-      </c>
-      <c r="I71">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="72" spans="1:9">
-      <c r="A72">
-        <v>34.36</v>
-      </c>
-      <c r="B72" t="s">
+        <v>99.98</v>
+      </c>
+      <c r="I69" t="s">
         <v>79</v>
-      </c>
-      <c r="C72" t="s">
-        <v>89</v>
-      </c>
-      <c r="D72" t="s">
-        <v>90</v>
-      </c>
-      <c r="E72">
-        <v>5.9</v>
-      </c>
-      <c r="F72">
-        <v>0.1717</v>
-      </c>
-      <c r="G72">
-        <v>0.14</v>
-      </c>
-      <c r="H72">
-        <v>96.59999999999999</v>
-      </c>
-      <c r="I72">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="73" spans="1:9">
-      <c r="A73">
-        <v>34.86</v>
-      </c>
-      <c r="B73" t="s">
-        <v>80</v>
-      </c>
-      <c r="C73" t="s">
-        <v>89</v>
-      </c>
-      <c r="D73" t="s">
-        <v>90</v>
-      </c>
-      <c r="E73">
-        <v>5.07</v>
-      </c>
-      <c r="F73">
-        <v>0.1454</v>
-      </c>
-      <c r="G73">
-        <v>0.15</v>
-      </c>
-      <c r="H73">
-        <v>97.37</v>
-      </c>
-      <c r="I73">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="74" spans="1:9">
-      <c r="A74">
-        <v>35.11</v>
-      </c>
-      <c r="B74" t="s">
-        <v>81</v>
-      </c>
-      <c r="C74" t="s">
-        <v>89</v>
-      </c>
-      <c r="D74" t="s">
-        <v>90</v>
-      </c>
-      <c r="E74">
-        <v>0</v>
-      </c>
-      <c r="F74">
-        <v>0</v>
-      </c>
-      <c r="G74">
-        <v>0.16</v>
-      </c>
-      <c r="H74">
-        <v>97.69</v>
-      </c>
-      <c r="I74">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="75" spans="1:9">
-      <c r="A75">
-        <v>35.61</v>
-      </c>
-      <c r="B75" t="s">
-        <v>82</v>
-      </c>
-      <c r="C75" t="s">
-        <v>89</v>
-      </c>
-      <c r="D75" t="s">
-        <v>90</v>
-      </c>
-      <c r="E75">
-        <v>6.25</v>
-      </c>
-      <c r="F75">
-        <v>0.1755</v>
-      </c>
-      <c r="G75">
-        <v>0.18</v>
-      </c>
-      <c r="H75">
-        <v>98.23</v>
-      </c>
-      <c r="I75">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="76" spans="1:9">
-      <c r="A76">
-        <v>36.86</v>
-      </c>
-      <c r="B76" t="s">
-        <v>83</v>
-      </c>
-      <c r="C76" t="s">
-        <v>89</v>
-      </c>
-      <c r="D76" t="s">
-        <v>90</v>
-      </c>
-      <c r="E76">
-        <v>0</v>
-      </c>
-      <c r="F76">
-        <v>0</v>
-      </c>
-      <c r="G76">
-        <v>0.22</v>
-      </c>
-      <c r="H76">
-        <v>99.12</v>
-      </c>
-      <c r="I76">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="77" spans="1:9">
-      <c r="A77">
-        <v>37.36</v>
-      </c>
-      <c r="B77" t="s">
-        <v>84</v>
-      </c>
-      <c r="C77" t="s">
-        <v>89</v>
-      </c>
-      <c r="D77" t="s">
-        <v>90</v>
-      </c>
-      <c r="E77">
-        <v>0</v>
-      </c>
-      <c r="F77">
-        <v>0</v>
-      </c>
-      <c r="G77">
-        <v>0.23</v>
-      </c>
-      <c r="H77">
-        <v>99.34</v>
-      </c>
-      <c r="I77">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="78" spans="1:9">
-      <c r="A78">
-        <v>37.86</v>
-      </c>
-      <c r="B78" t="s">
-        <v>85</v>
-      </c>
-      <c r="C78" t="s">
-        <v>89</v>
-      </c>
-      <c r="D78" t="s">
-        <v>90</v>
-      </c>
-      <c r="E78">
-        <v>0</v>
-      </c>
-      <c r="F78">
-        <v>0</v>
-      </c>
-      <c r="G78">
-        <v>0.25</v>
-      </c>
-      <c r="H78">
-        <v>99.51000000000001</v>
-      </c>
-      <c r="I78">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="79" spans="1:9">
-      <c r="A79">
-        <v>38.36</v>
-      </c>
-      <c r="B79" t="s">
-        <v>86</v>
-      </c>
-      <c r="C79" t="s">
-        <v>89</v>
-      </c>
-      <c r="D79" t="s">
-        <v>90</v>
-      </c>
-      <c r="E79">
-        <v>0</v>
-      </c>
-      <c r="F79">
-        <v>0</v>
-      </c>
-      <c r="G79">
-        <v>0.27</v>
-      </c>
-      <c r="H79">
-        <v>99.64</v>
-      </c>
-      <c r="I79">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="80" spans="1:9">
-      <c r="A80">
-        <v>38.86</v>
-      </c>
-      <c r="B80" t="s">
-        <v>87</v>
-      </c>
-      <c r="C80" t="s">
-        <v>89</v>
-      </c>
-      <c r="D80" t="s">
-        <v>90</v>
-      </c>
-      <c r="E80">
-        <v>0</v>
-      </c>
-      <c r="F80">
-        <v>0</v>
-      </c>
-      <c r="G80">
-        <v>0.28</v>
-      </c>
-      <c r="H80">
-        <v>99.73999999999999</v>
-      </c>
-      <c r="I80">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="81" spans="1:9">
-      <c r="A81">
-        <v>43.11</v>
-      </c>
-      <c r="B81" t="s">
-        <v>88</v>
-      </c>
-      <c r="C81" t="s">
-        <v>89</v>
-      </c>
-      <c r="D81" t="s">
-        <v>90</v>
-      </c>
-      <c r="E81" t="s">
-        <v>91</v>
-      </c>
-      <c r="G81">
-        <v>0.42</v>
-      </c>
-      <c r="H81">
-        <v>99.98</v>
-      </c>
-      <c r="I81" t="s">
-        <v>91</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
novo robo de noticia
</commit_message>
<xml_diff>
--- a/Robo_PUT_ITUB4.xlsx
+++ b/Robo_PUT_ITUB4.xlsx
@@ -669,7 +669,7 @@
         <v>0</v>
       </c>
       <c r="I2">
-        <v>0</v>
+        <v>1500</v>
       </c>
     </row>
     <row r="3" spans="1:9">
@@ -695,7 +695,7 @@
         <v>-0.38</v>
       </c>
       <c r="H3">
-        <v>0.12</v>
+        <v>0.2</v>
       </c>
       <c r="I3">
         <v>0</v>
@@ -724,7 +724,7 @@
         <v>-0.36</v>
       </c>
       <c r="H4">
-        <v>0.24</v>
+        <v>0.38</v>
       </c>
       <c r="I4">
         <v>0</v>
@@ -750,10 +750,10 @@
         <v>0.006</v>
       </c>
       <c r="G5">
-        <v>-0.34</v>
+        <v>-0.35</v>
       </c>
       <c r="H5">
-        <v>0.46</v>
+        <v>0.6899999999999999</v>
       </c>
       <c r="I5">
         <v>0</v>
@@ -773,19 +773,19 @@
         <v>78</v>
       </c>
       <c r="E6">
-        <v>0.02</v>
+        <v>0.01</v>
       </c>
       <c r="F6">
-        <v>0.001</v>
+        <v>0.0005</v>
       </c>
       <c r="G6">
         <v>-0.34</v>
       </c>
       <c r="H6">
-        <v>0.61</v>
+        <v>0.91</v>
       </c>
       <c r="I6">
-        <v>0</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="7" spans="1:9">
@@ -811,7 +811,7 @@
         <v>-0.33</v>
       </c>
       <c r="H7">
-        <v>0.8100000000000001</v>
+        <v>1.19</v>
       </c>
       <c r="I7">
         <v>0</v>
@@ -840,7 +840,7 @@
         <v>-0.32</v>
       </c>
       <c r="H8">
-        <v>1.06</v>
+        <v>1.53</v>
       </c>
       <c r="I8">
         <v>0</v>
@@ -869,7 +869,7 @@
         <v>-0.31</v>
       </c>
       <c r="H9">
-        <v>1.36</v>
+        <v>1.95</v>
       </c>
       <c r="I9">
         <v>0</v>
@@ -895,10 +895,10 @@
         <v>0.0033</v>
       </c>
       <c r="G10">
-        <v>-0.3</v>
+        <v>-0.31</v>
       </c>
       <c r="H10">
-        <v>1.74</v>
+        <v>2.46</v>
       </c>
       <c r="I10">
         <v>0</v>
@@ -927,7 +927,7 @@
         <v>-0.29</v>
       </c>
       <c r="H11">
-        <v>2.73</v>
+        <v>3.8</v>
       </c>
       <c r="I11">
         <v>0</v>
@@ -956,7 +956,7 @@
         <v>-0.28</v>
       </c>
       <c r="H12">
-        <v>3.37</v>
+        <v>4.64</v>
       </c>
       <c r="I12">
         <v>0</v>
@@ -985,10 +985,10 @@
         <v>-0.27</v>
       </c>
       <c r="H13">
-        <v>4.13</v>
+        <v>5.61</v>
       </c>
       <c r="I13">
-        <v>0</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="14" spans="1:9">
@@ -1011,10 +1011,10 @@
         <v>0.0036</v>
       </c>
       <c r="G14">
-        <v>-0.26</v>
+        <v>-0.27</v>
       </c>
       <c r="H14">
-        <v>5</v>
+        <v>6.73</v>
       </c>
       <c r="I14">
         <v>0</v>
@@ -1040,10 +1040,10 @@
         <v>0.0035</v>
       </c>
       <c r="G15">
-        <v>-0.25</v>
+        <v>-0.26</v>
       </c>
       <c r="H15">
-        <v>6</v>
+        <v>7.99</v>
       </c>
       <c r="I15">
         <v>0</v>
@@ -1069,10 +1069,10 @@
         <v>0.0061</v>
       </c>
       <c r="G16">
-        <v>-0.24</v>
+        <v>-0.25</v>
       </c>
       <c r="H16">
-        <v>7.14</v>
+        <v>9.41</v>
       </c>
       <c r="I16">
         <v>0</v>
@@ -1092,19 +1092,19 @@
         <v>78</v>
       </c>
       <c r="E17">
-        <v>0.1</v>
+        <v>0.07000000000000001</v>
       </c>
       <c r="F17">
-        <v>0.0043</v>
+        <v>0.003</v>
       </c>
       <c r="G17">
         <v>-0.24</v>
       </c>
       <c r="H17">
-        <v>8.42</v>
+        <v>10.99</v>
       </c>
       <c r="I17">
-        <v>0</v>
+        <v>2500</v>
       </c>
     </row>
     <row r="18" spans="1:9">
@@ -1121,19 +1121,19 @@
         <v>78</v>
       </c>
       <c r="E18">
-        <v>0.1</v>
+        <v>0.08</v>
       </c>
       <c r="F18">
-        <v>0.0043</v>
+        <v>0.0034</v>
       </c>
       <c r="G18">
         <v>-0.23</v>
       </c>
       <c r="H18">
-        <v>9.859999999999999</v>
+        <v>12.73</v>
       </c>
       <c r="I18">
-        <v>0</v>
+        <v>1200</v>
       </c>
     </row>
     <row r="19" spans="1:9">
@@ -1150,19 +1150,19 @@
         <v>78</v>
       </c>
       <c r="E19">
-        <v>0.12</v>
+        <v>0.08</v>
       </c>
       <c r="F19">
-        <v>0.0051</v>
+        <v>0.0034</v>
       </c>
       <c r="G19">
         <v>-0.22</v>
       </c>
       <c r="H19">
-        <v>11.44</v>
+        <v>14.63</v>
       </c>
       <c r="I19">
-        <v>0</v>
+        <v>2200</v>
       </c>
     </row>
     <row r="20" spans="1:9">
@@ -1179,19 +1179,19 @@
         <v>78</v>
       </c>
       <c r="E20">
-        <v>0.12</v>
+        <v>0.09</v>
       </c>
       <c r="F20">
-        <v>0.005</v>
+        <v>0.0038</v>
       </c>
       <c r="G20">
-        <v>-0.21</v>
+        <v>-0.22</v>
       </c>
       <c r="H20">
-        <v>13.18</v>
+        <v>16.69</v>
       </c>
       <c r="I20">
-        <v>0</v>
+        <v>2000</v>
       </c>
     </row>
     <row r="21" spans="1:9">
@@ -1208,19 +1208,19 @@
         <v>78</v>
       </c>
       <c r="E21">
-        <v>0.15</v>
+        <v>0.14</v>
       </c>
       <c r="F21">
-        <v>0.0062</v>
+        <v>0.0058</v>
       </c>
       <c r="G21">
-        <v>-0.2</v>
+        <v>-0.21</v>
       </c>
       <c r="H21">
-        <v>15.07</v>
+        <v>18.9</v>
       </c>
       <c r="I21">
-        <v>0</v>
+        <v>2000</v>
       </c>
     </row>
     <row r="22" spans="1:9">
@@ -1237,19 +1237,19 @@
         <v>78</v>
       </c>
       <c r="E22">
-        <v>0.18</v>
+        <v>0.12</v>
       </c>
       <c r="F22">
-        <v>0.0074</v>
+        <v>0.0049</v>
       </c>
       <c r="G22">
-        <v>-0.19</v>
+        <v>-0.2</v>
       </c>
       <c r="H22">
-        <v>17.11</v>
+        <v>21.26</v>
       </c>
       <c r="I22">
-        <v>0</v>
+        <v>100</v>
       </c>
     </row>
     <row r="23" spans="1:9">
@@ -1275,7 +1275,7 @@
         <v>-0.19</v>
       </c>
       <c r="H23">
-        <v>19.3</v>
+        <v>23.76</v>
       </c>
       <c r="I23">
         <v>0</v>
@@ -1295,19 +1295,19 @@
         <v>78</v>
       </c>
       <c r="E24">
-        <v>0.19</v>
+        <v>0.13</v>
       </c>
       <c r="F24">
-        <v>0.0076</v>
+        <v>0.0052</v>
       </c>
       <c r="G24">
         <v>-0.18</v>
       </c>
       <c r="H24">
-        <v>21.63</v>
+        <v>26.39</v>
       </c>
       <c r="I24">
-        <v>0</v>
+        <v>10000</v>
       </c>
     </row>
     <row r="25" spans="1:9">
@@ -1324,19 +1324,19 @@
         <v>78</v>
       </c>
       <c r="E25">
-        <v>0.21</v>
+        <v>0.19</v>
       </c>
       <c r="F25">
-        <v>0.008399999999999999</v>
+        <v>0.0076</v>
       </c>
       <c r="G25">
-        <v>-0.17</v>
+        <v>-0.18</v>
       </c>
       <c r="H25">
-        <v>24.08</v>
+        <v>29.12</v>
       </c>
       <c r="I25">
-        <v>0</v>
+        <v>11000</v>
       </c>
     </row>
     <row r="26" spans="1:9">
@@ -1359,13 +1359,13 @@
         <v>0.008699999999999999</v>
       </c>
       <c r="G26">
-        <v>-0.16</v>
+        <v>-0.17</v>
       </c>
       <c r="H26">
-        <v>26.66</v>
+        <v>31.96</v>
       </c>
       <c r="I26">
-        <v>0</v>
+        <v>2100</v>
       </c>
     </row>
     <row r="27" spans="1:9">
@@ -1382,19 +1382,19 @@
         <v>78</v>
       </c>
       <c r="E27">
-        <v>0.25</v>
+        <v>0.23</v>
       </c>
       <c r="F27">
-        <v>0.0098</v>
+        <v>0.008999999999999999</v>
       </c>
       <c r="G27">
-        <v>-0.15</v>
+        <v>-0.16</v>
       </c>
       <c r="H27">
-        <v>29.33</v>
+        <v>34.87</v>
       </c>
       <c r="I27">
-        <v>0</v>
+        <v>700</v>
       </c>
     </row>
     <row r="28" spans="1:9">
@@ -1411,19 +1411,19 @@
         <v>78</v>
       </c>
       <c r="E28">
-        <v>0.27</v>
+        <v>0.26</v>
       </c>
       <c r="F28">
-        <v>0.0104</v>
+        <v>0.0101</v>
       </c>
       <c r="G28">
         <v>-0.15</v>
       </c>
       <c r="H28">
-        <v>32.1</v>
+        <v>37.84</v>
       </c>
       <c r="I28">
-        <v>0</v>
+        <v>17600</v>
       </c>
     </row>
     <row r="29" spans="1:9">
@@ -1440,19 +1440,19 @@
         <v>78</v>
       </c>
       <c r="E29">
-        <v>0.3</v>
+        <v>0.29</v>
       </c>
       <c r="F29">
-        <v>0.0115</v>
+        <v>0.0111</v>
       </c>
       <c r="G29">
         <v>-0.14</v>
       </c>
       <c r="H29">
-        <v>34.95</v>
+        <v>40.86</v>
       </c>
       <c r="I29">
-        <v>0</v>
+        <v>101500</v>
       </c>
     </row>
     <row r="30" spans="1:9">
@@ -1469,19 +1469,19 @@
         <v>78</v>
       </c>
       <c r="E30">
-        <v>0.33</v>
+        <v>0.32</v>
       </c>
       <c r="F30">
-        <v>0.0125</v>
+        <v>0.0121</v>
       </c>
       <c r="G30">
         <v>-0.13</v>
       </c>
       <c r="H30">
-        <v>37.85</v>
+        <v>43.91</v>
       </c>
       <c r="I30">
-        <v>0</v>
+        <v>116900</v>
       </c>
     </row>
     <row r="31" spans="1:9">
@@ -1498,19 +1498,19 @@
         <v>78</v>
       </c>
       <c r="E31">
-        <v>0.37</v>
+        <v>0.36</v>
       </c>
       <c r="F31">
-        <v>0.0139</v>
+        <v>0.0135</v>
       </c>
       <c r="G31">
-        <v>-0.12</v>
+        <v>-0.13</v>
       </c>
       <c r="H31">
-        <v>40.79</v>
+        <v>46.96</v>
       </c>
       <c r="I31">
-        <v>0</v>
+        <v>140800</v>
       </c>
     </row>
     <row r="32" spans="1:9">
@@ -1527,19 +1527,19 @@
         <v>78</v>
       </c>
       <c r="E32">
-        <v>0.41</v>
+        <v>0.37</v>
       </c>
       <c r="F32">
-        <v>0.0153</v>
+        <v>0.0138</v>
       </c>
       <c r="G32">
-        <v>-0.11</v>
+        <v>-0.12</v>
       </c>
       <c r="H32">
-        <v>43.76</v>
+        <v>50</v>
       </c>
       <c r="I32">
-        <v>0</v>
+        <v>156600</v>
       </c>
     </row>
     <row r="33" spans="1:9">
@@ -1556,19 +1556,19 @@
         <v>78</v>
       </c>
       <c r="E33">
-        <v>0.47</v>
+        <v>0.44</v>
       </c>
       <c r="F33">
-        <v>0.0173</v>
+        <v>0.0162</v>
       </c>
       <c r="G33">
-        <v>-0.1</v>
+        <v>-0.11</v>
       </c>
       <c r="H33">
-        <v>46.74</v>
+        <v>53.02</v>
       </c>
       <c r="I33">
-        <v>0</v>
+        <v>149800</v>
       </c>
     </row>
     <row r="34" spans="1:9">
@@ -1585,19 +1585,19 @@
         <v>78</v>
       </c>
       <c r="E34">
-        <v>0.53</v>
+        <v>0.47</v>
       </c>
       <c r="F34">
-        <v>0.0194</v>
+        <v>0.0172</v>
       </c>
       <c r="G34">
         <v>-0.1</v>
       </c>
       <c r="H34">
-        <v>49.71</v>
+        <v>55.98</v>
       </c>
       <c r="I34">
-        <v>0</v>
+        <v>248900</v>
       </c>
     </row>
     <row r="35" spans="1:9">
@@ -1614,19 +1614,19 @@
         <v>78</v>
       </c>
       <c r="E35">
-        <v>0.57</v>
+        <v>0.43</v>
       </c>
       <c r="F35">
-        <v>0.0206</v>
+        <v>0.0156</v>
       </c>
       <c r="G35">
         <v>-0.09</v>
       </c>
       <c r="H35">
-        <v>52.65</v>
+        <v>58.89</v>
       </c>
       <c r="I35">
-        <v>0</v>
+        <v>132500</v>
       </c>
     </row>
     <row r="36" spans="1:9">
@@ -1643,19 +1643,19 @@
         <v>78</v>
       </c>
       <c r="E36">
-        <v>0.59</v>
+        <v>0.5600000000000001</v>
       </c>
       <c r="F36">
-        <v>0.0212</v>
+        <v>0.0201</v>
       </c>
       <c r="G36">
         <v>-0.08</v>
       </c>
       <c r="H36">
-        <v>55.55</v>
+        <v>61.73</v>
       </c>
       <c r="I36">
-        <v>0</v>
+        <v>142400</v>
       </c>
     </row>
     <row r="37" spans="1:9">
@@ -1678,13 +1678,13 @@
         <v>0.0235</v>
       </c>
       <c r="G37">
-        <v>-0.07000000000000001</v>
+        <v>-0.08</v>
       </c>
       <c r="H37">
-        <v>58.4</v>
+        <v>64.48</v>
       </c>
       <c r="I37">
-        <v>0</v>
+        <v>232200</v>
       </c>
     </row>
     <row r="38" spans="1:9">
@@ -1701,19 +1701,19 @@
         <v>78</v>
       </c>
       <c r="E38">
-        <v>0.76</v>
+        <v>0.72</v>
       </c>
       <c r="F38">
-        <v>0.0268</v>
+        <v>0.0254</v>
       </c>
       <c r="G38">
-        <v>-0.06</v>
+        <v>-0.07000000000000001</v>
       </c>
       <c r="H38">
-        <v>61.18</v>
+        <v>67.13</v>
       </c>
       <c r="I38">
-        <v>0</v>
+        <v>177400</v>
       </c>
     </row>
     <row r="39" spans="1:9">
@@ -1730,19 +1730,19 @@
         <v>78</v>
       </c>
       <c r="E39">
-        <v>0.83</v>
+        <v>0.79</v>
       </c>
       <c r="F39">
-        <v>0.029</v>
+        <v>0.0276</v>
       </c>
       <c r="G39">
-        <v>-0.05</v>
+        <v>-0.06</v>
       </c>
       <c r="H39">
-        <v>63.88</v>
+        <v>69.68000000000001</v>
       </c>
       <c r="I39">
-        <v>0</v>
+        <v>61600</v>
       </c>
     </row>
     <row r="40" spans="1:9">
@@ -1759,19 +1759,19 @@
         <v>78</v>
       </c>
       <c r="E40">
-        <v>0.9</v>
+        <v>0.87</v>
       </c>
       <c r="F40">
-        <v>0.0312</v>
+        <v>0.0301</v>
       </c>
       <c r="G40">
         <v>-0.05</v>
       </c>
       <c r="H40">
-        <v>66.48999999999999</v>
+        <v>72.11</v>
       </c>
       <c r="I40">
-        <v>0</v>
+        <v>190600</v>
       </c>
     </row>
     <row r="41" spans="1:9">
@@ -1788,19 +1788,19 @@
         <v>78</v>
       </c>
       <c r="E41">
-        <v>0.97</v>
+        <v>0.96</v>
       </c>
       <c r="F41">
-        <v>0.0333</v>
+        <v>0.033</v>
       </c>
       <c r="G41">
         <v>-0.04</v>
       </c>
       <c r="H41">
-        <v>69</v>
+        <v>74.43000000000001</v>
       </c>
       <c r="I41">
-        <v>0</v>
+        <v>46500</v>
       </c>
     </row>
     <row r="42" spans="1:9">
@@ -1817,19 +1817,19 @@
         <v>78</v>
       </c>
       <c r="E42">
-        <v>1.15</v>
+        <v>1.01</v>
       </c>
       <c r="F42">
-        <v>0.0392</v>
+        <v>0.0344</v>
       </c>
       <c r="G42">
-        <v>-0.03</v>
+        <v>-0.04</v>
       </c>
       <c r="H42">
-        <v>71.40000000000001</v>
+        <v>76.62</v>
       </c>
       <c r="I42">
-        <v>0</v>
+        <v>62200</v>
       </c>
     </row>
     <row r="43" spans="1:9">
@@ -1846,19 +1846,19 @@
         <v>78</v>
       </c>
       <c r="E43">
-        <v>1.18</v>
+        <v>1.11</v>
       </c>
       <c r="F43">
-        <v>0.0399</v>
+        <v>0.0375</v>
       </c>
       <c r="G43">
-        <v>-0.02</v>
+        <v>-0.03</v>
       </c>
       <c r="H43">
-        <v>73.69</v>
+        <v>78.69</v>
       </c>
       <c r="I43">
-        <v>0</v>
+        <v>28500</v>
       </c>
     </row>
     <row r="44" spans="1:9">
@@ -1875,19 +1875,19 @@
         <v>78</v>
       </c>
       <c r="E44">
-        <v>1.26</v>
+        <v>1.24</v>
       </c>
       <c r="F44">
-        <v>0.0422</v>
+        <v>0.0415</v>
       </c>
       <c r="G44">
-        <v>-0.01</v>
+        <v>-0.02</v>
       </c>
       <c r="H44">
-        <v>75.87</v>
+        <v>80.63</v>
       </c>
       <c r="I44">
-        <v>0</v>
+        <v>395100</v>
       </c>
     </row>
     <row r="45" spans="1:9">
@@ -1904,19 +1904,19 @@
         <v>78</v>
       </c>
       <c r="E45">
-        <v>1.38</v>
+        <v>1.33</v>
       </c>
       <c r="F45">
-        <v>0.0458</v>
+        <v>0.0442</v>
       </c>
       <c r="G45">
-        <v>-0</v>
+        <v>-0.01</v>
       </c>
       <c r="H45">
-        <v>77.93000000000001</v>
+        <v>82.44</v>
       </c>
       <c r="I45">
-        <v>0</v>
+        <v>41800</v>
       </c>
     </row>
     <row r="46" spans="1:9">
@@ -1933,19 +1933,19 @@
         <v>78</v>
       </c>
       <c r="E46">
-        <v>1.48</v>
+        <v>1.29</v>
       </c>
       <c r="F46">
-        <v>0.0487</v>
+        <v>0.0425</v>
       </c>
       <c r="G46">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="H46">
-        <v>79.87</v>
+        <v>84.13</v>
       </c>
       <c r="I46">
-        <v>0</v>
+        <v>40800</v>
       </c>
     </row>
     <row r="47" spans="1:9">
@@ -1962,19 +1962,19 @@
         <v>78</v>
       </c>
       <c r="E47">
-        <v>1.6</v>
+        <v>1.35</v>
       </c>
       <c r="F47">
-        <v>0.0523</v>
+        <v>0.0441</v>
       </c>
       <c r="G47">
         <v>0.01</v>
       </c>
       <c r="H47">
-        <v>81.69</v>
+        <v>85.69</v>
       </c>
       <c r="I47">
-        <v>0</v>
+        <v>10700</v>
       </c>
     </row>
     <row r="48" spans="1:9">
@@ -1991,19 +1991,19 @@
         <v>78</v>
       </c>
       <c r="E48">
-        <v>1.75</v>
+        <v>1.66</v>
       </c>
       <c r="F48">
-        <v>0.0567</v>
+        <v>0.0538</v>
       </c>
       <c r="G48">
-        <v>0.02</v>
+        <v>0.01</v>
       </c>
       <c r="H48">
-        <v>83.38</v>
+        <v>87.14</v>
       </c>
       <c r="I48">
-        <v>0</v>
+        <v>761000</v>
       </c>
     </row>
     <row r="49" spans="1:9">
@@ -2020,19 +2020,19 @@
         <v>78</v>
       </c>
       <c r="E49">
-        <v>1.99</v>
+        <v>1.63</v>
       </c>
       <c r="F49">
-        <v>0.064</v>
+        <v>0.0524</v>
       </c>
       <c r="G49">
-        <v>0.03</v>
+        <v>0.02</v>
       </c>
       <c r="H49">
-        <v>84.97</v>
+        <v>88.47</v>
       </c>
       <c r="I49">
-        <v>0</v>
+        <v>189900</v>
       </c>
     </row>
     <row r="50" spans="1:9">
@@ -2049,19 +2049,19 @@
         <v>78</v>
       </c>
       <c r="E50">
-        <v>2.1</v>
+        <v>1.82</v>
       </c>
       <c r="F50">
-        <v>0.067</v>
+        <v>0.058</v>
       </c>
       <c r="G50">
-        <v>0.04</v>
+        <v>0.03</v>
       </c>
       <c r="H50">
-        <v>86.43000000000001</v>
+        <v>89.69</v>
       </c>
       <c r="I50">
-        <v>0</v>
+        <v>34900</v>
       </c>
     </row>
     <row r="51" spans="1:9">
@@ -2078,19 +2078,19 @@
         <v>78</v>
       </c>
       <c r="E51">
-        <v>2.22</v>
+        <v>2.12</v>
       </c>
       <c r="F51">
-        <v>0.0702</v>
+        <v>0.06710000000000001</v>
       </c>
       <c r="G51">
         <v>0.04</v>
       </c>
       <c r="H51">
-        <v>87.79000000000001</v>
+        <v>90.81</v>
       </c>
       <c r="I51">
-        <v>0</v>
+        <v>45900</v>
       </c>
     </row>
     <row r="52" spans="1:9">
@@ -2107,19 +2107,19 @@
         <v>78</v>
       </c>
       <c r="E52">
-        <v>2.6</v>
+        <v>2.01</v>
       </c>
       <c r="F52">
-        <v>0.08160000000000001</v>
+        <v>0.0631</v>
       </c>
       <c r="G52">
         <v>0.05</v>
       </c>
       <c r="H52">
-        <v>89.03</v>
+        <v>91.81999999999999</v>
       </c>
       <c r="I52">
-        <v>0</v>
+        <v>15800</v>
       </c>
     </row>
     <row r="53" spans="1:9">
@@ -2136,19 +2136,19 @@
         <v>78</v>
       </c>
       <c r="E53">
-        <v>2.41</v>
+        <v>2.12</v>
       </c>
       <c r="F53">
-        <v>0.0751</v>
+        <v>0.066</v>
       </c>
       <c r="G53">
-        <v>0.06</v>
+        <v>0.05</v>
       </c>
       <c r="H53">
-        <v>90.18000000000001</v>
+        <v>92.75</v>
       </c>
       <c r="I53">
-        <v>0</v>
+        <v>600</v>
       </c>
     </row>
     <row r="54" spans="1:9">
@@ -2165,19 +2165,19 @@
         <v>78</v>
       </c>
       <c r="E54">
-        <v>2.88</v>
+        <v>2.25</v>
       </c>
       <c r="F54">
-        <v>0.089</v>
+        <v>0.06950000000000001</v>
       </c>
       <c r="G54">
-        <v>0.07000000000000001</v>
+        <v>0.06</v>
       </c>
       <c r="H54">
-        <v>91.22</v>
+        <v>93.58</v>
       </c>
       <c r="I54">
-        <v>0</v>
+        <v>400</v>
       </c>
     </row>
     <row r="55" spans="1:9">
@@ -2200,10 +2200,10 @@
         <v>0.2364</v>
       </c>
       <c r="G55">
-        <v>0.08</v>
+        <v>0.07000000000000001</v>
       </c>
       <c r="H55">
-        <v>92.18000000000001</v>
+        <v>94.33</v>
       </c>
       <c r="I55">
         <v>0</v>
@@ -2229,10 +2229,10 @@
         <v>0.1035</v>
       </c>
       <c r="G56">
-        <v>0.09</v>
+        <v>0.08</v>
       </c>
       <c r="H56">
-        <v>93.04000000000001</v>
+        <v>95.01000000000001</v>
       </c>
       <c r="I56">
         <v>0</v>
@@ -2252,19 +2252,19 @@
         <v>78</v>
       </c>
       <c r="E57">
-        <v>0</v>
+        <v>2.8</v>
       </c>
       <c r="F57">
-        <v>0</v>
+        <v>0.08459999999999999</v>
       </c>
       <c r="G57">
         <v>0.09</v>
       </c>
       <c r="H57">
-        <v>93.83</v>
+        <v>95.61</v>
       </c>
       <c r="I57">
-        <v>0</v>
+        <v>8800</v>
       </c>
     </row>
     <row r="58" spans="1:9">
@@ -2287,10 +2287,10 @@
         <v>0</v>
       </c>
       <c r="G58">
-        <v>0.11</v>
+        <v>0.1</v>
       </c>
       <c r="H58">
-        <v>95.18000000000001</v>
+        <v>96.64</v>
       </c>
       <c r="I58">
         <v>0</v>
@@ -2316,10 +2316,10 @@
         <v>0</v>
       </c>
       <c r="G59">
-        <v>0.13</v>
+        <v>0.12</v>
       </c>
       <c r="H59">
-        <v>96.26000000000001</v>
+        <v>97.44</v>
       </c>
       <c r="I59">
         <v>0</v>
@@ -2345,10 +2345,10 @@
         <v>0.1717</v>
       </c>
       <c r="G60">
-        <v>0.14</v>
+        <v>0.13</v>
       </c>
       <c r="H60">
-        <v>96.72</v>
+        <v>97.78</v>
       </c>
       <c r="I60">
         <v>0</v>
@@ -2377,7 +2377,7 @@
         <v>0.15</v>
       </c>
       <c r="H61">
-        <v>97.48999999999999</v>
+        <v>98.33</v>
       </c>
       <c r="I61">
         <v>0</v>
@@ -2403,10 +2403,10 @@
         <v>0</v>
       </c>
       <c r="G62">
-        <v>0.16</v>
+        <v>0.15</v>
       </c>
       <c r="H62">
-        <v>97.81</v>
+        <v>98.56</v>
       </c>
       <c r="I62">
         <v>0</v>
@@ -2432,10 +2432,10 @@
         <v>0.1488</v>
       </c>
       <c r="G63">
-        <v>0.18</v>
+        <v>0.17</v>
       </c>
       <c r="H63">
-        <v>98.34999999999999</v>
+        <v>98.93000000000001</v>
       </c>
       <c r="I63">
         <v>0</v>
@@ -2461,10 +2461,10 @@
         <v>0</v>
       </c>
       <c r="G64">
-        <v>0.22</v>
+        <v>0.21</v>
       </c>
       <c r="H64">
-        <v>99.2</v>
+        <v>99.51000000000001</v>
       </c>
       <c r="I64">
         <v>0</v>
@@ -2493,7 +2493,7 @@
         <v>0.23</v>
       </c>
       <c r="H65">
-        <v>99.41</v>
+        <v>99.65000000000001</v>
       </c>
       <c r="I65">
         <v>0</v>
@@ -2519,10 +2519,10 @@
         <v>0</v>
       </c>
       <c r="G66">
-        <v>0.25</v>
+        <v>0.24</v>
       </c>
       <c r="H66">
-        <v>99.56999999999999</v>
+        <v>99.75</v>
       </c>
       <c r="I66">
         <v>0</v>
@@ -2548,10 +2548,10 @@
         <v>0</v>
       </c>
       <c r="G67">
-        <v>0.27</v>
+        <v>0.26</v>
       </c>
       <c r="H67">
-        <v>99.69</v>
+        <v>99.81999999999999</v>
       </c>
       <c r="I67">
         <v>0</v>
@@ -2580,7 +2580,7 @@
         <v>0.28</v>
       </c>
       <c r="H68">
-        <v>99.77</v>
+        <v>99.87</v>
       </c>
       <c r="I68">
         <v>0</v>

</xml_diff>